<commit_message>
Changes to order model
</commit_message>
<xml_diff>
--- a/burndown template(4).xlsx
+++ b/burndown template(4).xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaari\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexander\Documents\GitHub\ifb299\IFB299-Team96\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9DB94AFD-790A-48AC-9386-C3934FEA468F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C2330DCB-5C70-4F8E-9D80-094334CCE7D5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{17158905-1468-4D0B-BDC3-3B4525E874D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Burn down chart" sheetId="2" r:id="rId1"/>
@@ -346,6 +346,11 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -357,11 +362,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1743,7 +1743,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-AU"/>
-              <a:t>Sprint 1 Burn</a:t>
+              <a:t>Sprint 2 Burn</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-AU" baseline="0"/>
@@ -1821,6 +1821,93 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Burn down chart'!$A$52:$A$77</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'Burn down chart'!$B$52:$B$87</c:f>
@@ -1959,6 +2046,93 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="0"/>
           </c:trendline>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Burn down chart'!$A$52:$A$77</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'Burn down chart'!$C$52:$C$87</c:f>
@@ -2000,6 +2174,27 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2092,7 +2287,7 @@
           </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -4082,13 +4277,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>827942</xdr:colOff>
+      <xdr:colOff>827941</xdr:colOff>
       <xdr:row>49</xdr:row>
       <xdr:rowOff>153865</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1580416</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1886138</xdr:colOff>
       <xdr:row>64</xdr:row>
       <xdr:rowOff>68873</xdr:rowOff>
     </xdr:to>
@@ -4385,28 +4580,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B51" zoomScale="101" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E70" sqref="E70"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="29.83203125" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="29.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="29.83203125" style="1"/>
-    <col min="3" max="3" width="26.71875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.27734375" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="29.83203125" style="1"/>
+    <col min="1" max="2" width="29.85546875" style="1"/>
+    <col min="3" max="3" width="26.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="29.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="14.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -4417,7 +4612,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -4428,7 +4623,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -4439,7 +4634,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -4447,34 +4642,34 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B6" s="3"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B8" s="11" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B8" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A11" s="10" t="s">
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -4485,7 +4680,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>35</v>
       </c>
@@ -4500,7 +4695,7 @@
         <v>43329</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>34</v>
       </c>
@@ -4515,7 +4710,7 @@
         <v>43330</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>33</v>
       </c>
@@ -4530,7 +4725,7 @@
         <v>43331</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>32</v>
       </c>
@@ -4545,7 +4740,7 @@
         <v>43332</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>31</v>
       </c>
@@ -4560,7 +4755,7 @@
         <v>43333</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>30</v>
       </c>
@@ -4575,7 +4770,7 @@
         <v>43334</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>29</v>
       </c>
@@ -4590,7 +4785,7 @@
         <v>43335</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>28</v>
       </c>
@@ -4605,7 +4800,7 @@
         <v>43336</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>27</v>
       </c>
@@ -4620,7 +4815,7 @@
         <v>43337</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>26</v>
       </c>
@@ -4635,7 +4830,7 @@
         <v>43338</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>25</v>
       </c>
@@ -4650,7 +4845,7 @@
         <v>43339</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>24</v>
       </c>
@@ -4665,7 +4860,7 @@
         <v>43340</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -4680,7 +4875,7 @@
         <v>43341</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>22</v>
       </c>
@@ -4695,7 +4890,7 @@
         <v>43342</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>21</v>
       </c>
@@ -4711,7 +4906,7 @@
         <v>43343</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>20</v>
       </c>
@@ -4727,7 +4922,7 @@
         <v>43344</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>19</v>
       </c>
@@ -4743,7 +4938,7 @@
         <v>43345</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>18</v>
       </c>
@@ -4759,7 +4954,7 @@
         <v>43346</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>17</v>
       </c>
@@ -4774,7 +4969,7 @@
         <v>43347</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>16</v>
       </c>
@@ -4789,7 +4984,7 @@
         <v>43348</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>15</v>
       </c>
@@ -4804,7 +4999,7 @@
         <v>43349</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>14</v>
       </c>
@@ -4819,7 +5014,7 @@
         <v>43350</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>13</v>
       </c>
@@ -4837,7 +5032,7 @@
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>12</v>
       </c>
@@ -4856,7 +5051,7 @@
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>11</v>
       </c>
@@ -4875,7 +5070,7 @@
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>10</v>
       </c>
@@ -4894,7 +5089,7 @@
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>9</v>
       </c>
@@ -4913,7 +5108,7 @@
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>8</v>
       </c>
@@ -4932,7 +5127,7 @@
       <c r="H40" s="6"/>
       <c r="I40" s="6"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>7</v>
       </c>
@@ -4951,7 +5146,7 @@
       <c r="H41" s="6"/>
       <c r="I41" s="6"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>6</v>
       </c>
@@ -4970,7 +5165,7 @@
       <c r="H42" s="6"/>
       <c r="I42" s="6"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>5</v>
       </c>
@@ -4989,7 +5184,7 @@
       <c r="H43" s="6"/>
       <c r="I43" s="6"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>4</v>
       </c>
@@ -5008,7 +5203,7 @@
       <c r="H44" s="6"/>
       <c r="I44" s="6"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>3</v>
       </c>
@@ -5027,7 +5222,7 @@
       <c r="H45" s="6"/>
       <c r="I45" s="6"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>2</v>
       </c>
@@ -5046,7 +5241,7 @@
       <c r="H46" s="6"/>
       <c r="I46" s="6"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>1</v>
       </c>
@@ -5065,7 +5260,7 @@
       <c r="H47" s="6"/>
       <c r="I47" s="6"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>0</v>
       </c>
@@ -5084,24 +5279,24 @@
       <c r="H48" s="6"/>
       <c r="I48" s="6"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
       <c r="H49" s="6"/>
       <c r="I49" s="6"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A50" s="10" t="s">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="B50" s="10"/>
-      <c r="C50" s="10"/>
+      <c r="B50" s="13"/>
+      <c r="C50" s="13"/>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
       <c r="H50" s="6"/>
       <c r="I50" s="6"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>0</v>
       </c>
@@ -5116,7 +5311,7 @@
       <c r="H51" s="6"/>
       <c r="I51" s="6"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>25</v>
       </c>
@@ -5134,7 +5329,7 @@
       <c r="H52" s="6"/>
       <c r="I52" s="6"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>24</v>
       </c>
@@ -5153,7 +5348,7 @@
       <c r="H53" s="6"/>
       <c r="I53" s="6"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>23</v>
       </c>
@@ -5172,7 +5367,7 @@
       <c r="H54" s="6"/>
       <c r="I54" s="6"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>22</v>
       </c>
@@ -5191,7 +5386,7 @@
       <c r="H55" s="6"/>
       <c r="I55" s="6"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>21</v>
       </c>
@@ -5210,7 +5405,7 @@
       <c r="H56" s="6"/>
       <c r="I56" s="6"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>20</v>
       </c>
@@ -5229,7 +5424,7 @@
       <c r="H57" s="6"/>
       <c r="I57" s="6"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>19</v>
       </c>
@@ -5248,7 +5443,7 @@
       <c r="H58" s="6"/>
       <c r="I58" s="6"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>18</v>
       </c>
@@ -5267,7 +5462,7 @@
       <c r="H59" s="6"/>
       <c r="I59" s="6"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>17</v>
       </c>
@@ -5286,7 +5481,7 @@
       <c r="H60" s="6"/>
       <c r="I60" s="6"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>16</v>
       </c>
@@ -5305,7 +5500,7 @@
       <c r="H61" s="6"/>
       <c r="I61" s="6"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>15</v>
       </c>
@@ -5324,7 +5519,7 @@
       <c r="H62" s="6"/>
       <c r="I62" s="6"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>14</v>
       </c>
@@ -5343,13 +5538,16 @@
       <c r="H63" s="6"/>
       <c r="I63" s="6"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>13</v>
       </c>
       <c r="B64" s="1">
         <f t="shared" si="1"/>
         <v>23</v>
+      </c>
+      <c r="C64" s="1">
+        <v>34</v>
       </c>
       <c r="D64" s="2">
         <v>43386</v>
@@ -5359,13 +5557,16 @@
       <c r="H64" s="6"/>
       <c r="I64" s="6"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>12</v>
       </c>
       <c r="B65" s="1">
         <f t="shared" si="1"/>
         <v>22</v>
+      </c>
+      <c r="C65" s="1">
+        <v>32</v>
       </c>
       <c r="D65" s="2">
         <v>43387</v>
@@ -5375,13 +5576,16 @@
       <c r="H65" s="6"/>
       <c r="I65" s="6"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>11</v>
       </c>
       <c r="B66" s="1">
         <f t="shared" si="1"/>
         <v>20</v>
+      </c>
+      <c r="C66" s="1">
+        <v>30</v>
       </c>
       <c r="D66" s="2">
         <v>43388</v>
@@ -5391,13 +5595,16 @@
       <c r="H66" s="6"/>
       <c r="I66" s="6"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>10</v>
       </c>
       <c r="B67" s="1">
         <f t="shared" si="1"/>
         <v>18</v>
+      </c>
+      <c r="C67" s="1">
+        <v>25</v>
       </c>
       <c r="D67" s="2">
         <v>43389</v>
@@ -5407,13 +5614,16 @@
       <c r="H67" s="6"/>
       <c r="I67" s="6"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>9</v>
       </c>
       <c r="B68" s="1">
         <f t="shared" si="1"/>
         <v>16</v>
+      </c>
+      <c r="C68" s="1">
+        <v>22</v>
       </c>
       <c r="D68" s="2">
         <v>43390</v>
@@ -5423,13 +5633,16 @@
       <c r="H68" s="6"/>
       <c r="I68" s="6"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>8</v>
       </c>
       <c r="B69" s="1">
         <f t="shared" si="1"/>
         <v>14</v>
+      </c>
+      <c r="C69" s="1">
+        <v>19</v>
       </c>
       <c r="D69" s="2">
         <v>43391</v>
@@ -5439,13 +5652,16 @@
       <c r="H69" s="6"/>
       <c r="I69" s="6"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>7</v>
       </c>
       <c r="B70" s="1">
         <f t="shared" si="1"/>
         <v>13</v>
+      </c>
+      <c r="C70" s="1">
+        <v>17</v>
       </c>
       <c r="D70" s="2">
         <v>43392</v>
@@ -5455,7 +5671,7 @@
       <c r="H70" s="6"/>
       <c r="I70" s="6"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>6</v>
       </c>
@@ -5471,7 +5687,7 @@
       <c r="H71" s="6"/>
       <c r="I71" s="6"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>5</v>
       </c>
@@ -5487,7 +5703,7 @@
       <c r="H72" s="6"/>
       <c r="I72" s="6"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>4</v>
       </c>
@@ -5499,7 +5715,7 @@
         <v>43395</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>3</v>
       </c>
@@ -5511,7 +5727,7 @@
         <v>43396</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>2</v>
       </c>
@@ -5523,7 +5739,7 @@
         <v>43397</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>1</v>
       </c>
@@ -5535,7 +5751,7 @@
         <v>43398</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>0</v>
       </c>
@@ -5547,84 +5763,84 @@
         <v>43399</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D78" s="2"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D79" s="2"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D80" s="2"/>
     </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.4">
+    <row r="81" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D81" s="2"/>
     </row>
-    <row r="82" spans="4:4" x14ac:dyDescent="0.4">
+    <row r="82" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D82" s="2"/>
     </row>
-    <row r="83" spans="4:4" x14ac:dyDescent="0.4">
+    <row r="83" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D83" s="2"/>
     </row>
-    <row r="84" spans="4:4" x14ac:dyDescent="0.4">
+    <row r="84" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D84" s="2"/>
     </row>
-    <row r="85" spans="4:4" x14ac:dyDescent="0.4">
+    <row r="85" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D85" s="2"/>
     </row>
-    <row r="86" spans="4:4" x14ac:dyDescent="0.4">
+    <row r="86" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D86" s="2"/>
     </row>
-    <row r="87" spans="4:4" x14ac:dyDescent="0.4">
+    <row r="87" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D87" s="2"/>
     </row>
-    <row r="101" spans="1:4" ht="14.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A101" s="8"/>
-      <c r="B101" s="9"/>
-      <c r="C101" s="9"/>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A101" s="11"/>
+      <c r="B101" s="12"/>
+      <c r="C101" s="12"/>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D103" s="2"/>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D104" s="2"/>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D105" s="2"/>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D106" s="2"/>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D107" s="2"/>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D108" s="2"/>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D109" s="2"/>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D110" s="2"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D111" s="2"/>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D112" s="2"/>
     </row>
-    <row r="113" spans="4:4" x14ac:dyDescent="0.4">
+    <row r="113" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D113" s="2"/>
     </row>
-    <row r="114" spans="4:4" x14ac:dyDescent="0.4">
+    <row r="114" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D114" s="2"/>
     </row>
-    <row r="115" spans="4:4" x14ac:dyDescent="0.4">
+    <row r="115" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D115" s="2"/>
     </row>
-    <row r="116" spans="4:4" x14ac:dyDescent="0.4">
+    <row r="116" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D116" s="2"/>
     </row>
-    <row r="117" spans="4:4" x14ac:dyDescent="0.4">
+    <row r="117" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D117" s="2"/>
     </row>
   </sheetData>
@@ -5650,18 +5866,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{509F8D58-4987-4C0A-AB6D-0E47BD987F94}">
   <dimension ref="A1:F72"/>
   <sheetViews>
-    <sheetView zoomScale="89" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.1640625" customWidth="1"/>
-    <col min="2" max="2" width="75.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="75.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.71875" customWidth="1"/>
+    <col min="5" max="5" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>17</v>
       </c>
@@ -5670,7 +5888,7 @@
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -5687,7 +5905,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -5705,7 +5923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -5723,7 +5941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -5736,7 +5954,7 @@
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -5749,7 +5967,7 @@
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="5" t="s">
         <v>16</v>
@@ -5760,7 +5978,7 @@
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
@@ -5769,7 +5987,7 @@
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
@@ -5786,7 +6004,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>1</v>
       </c>
@@ -5805,7 +6023,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>2</v>
       </c>
@@ -5824,7 +6042,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>3</v>
       </c>
@@ -5842,7 +6060,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>4</v>
       </c>
@@ -5855,7 +6073,7 @@
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>5</v>
       </c>
@@ -5868,7 +6086,7 @@
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="5" t="s">
         <v>16</v>
@@ -5879,7 +6097,7 @@
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>23</v>
       </c>
@@ -5888,7 +6106,7 @@
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>8</v>
       </c>
@@ -5905,7 +6123,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>1</v>
       </c>
@@ -5923,7 +6141,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>2</v>
       </c>
@@ -5941,7 +6159,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>3</v>
       </c>
@@ -5959,7 +6177,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>4</v>
       </c>
@@ -5972,7 +6190,7 @@
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="5" t="s">
         <v>27</v>
@@ -5983,7 +6201,7 @@
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
     </row>
-    <row r="23" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>28</v>
       </c>
@@ -5992,7 +6210,7 @@
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
     </row>
-    <row r="24" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>8</v>
       </c>
@@ -6009,7 +6227,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>1</v>
       </c>
@@ -6022,7 +6240,7 @@
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
     </row>
-    <row r="26" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>2</v>
       </c>
@@ -6035,7 +6253,7 @@
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
     </row>
-    <row r="27" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>3</v>
       </c>
@@ -6048,7 +6266,7 @@
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
     </row>
-    <row r="28" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="5" t="s">
         <v>30</v>
@@ -6059,7 +6277,7 @@
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
     </row>
-    <row r="29" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>31</v>
       </c>
@@ -6068,7 +6286,7 @@
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
     </row>
-    <row r="30" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>8</v>
       </c>
@@ -6085,7 +6303,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>1</v>
       </c>
@@ -6104,7 +6322,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>2</v>
       </c>
@@ -6117,7 +6335,7 @@
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
     </row>
-    <row r="33" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>3</v>
       </c>
@@ -6130,7 +6348,7 @@
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
     </row>
-    <row r="34" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>4</v>
       </c>
@@ -6143,11 +6361,11 @@
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
     </row>
-    <row r="35" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>5</v>
       </c>
-      <c r="B35" s="13" t="s">
+      <c r="B35" s="9" t="s">
         <v>15</v>
       </c>
       <c r="C35" s="5">
@@ -6156,7 +6374,7 @@
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
     </row>
-    <row r="36" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="B36" s="5" t="s">
         <v>30</v>
@@ -6167,7 +6385,7 @@
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E37" s="7" t="s">
         <v>38</v>
       </c>
@@ -6176,8 +6394,8 @@
         <v>10.799999999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="12" t="s">
+    <row r="39" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
         <v>47</v>
       </c>
       <c r="B39" s="4"/>
@@ -6185,7 +6403,7 @@
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
     </row>
-    <row r="40" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>8</v>
       </c>
@@ -6202,11 +6420,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>1</v>
       </c>
-      <c r="B41" s="13" t="s">
+      <c r="B41" s="9" t="s">
         <v>48</v>
       </c>
       <c r="C41" s="5">
@@ -6214,12 +6432,15 @@
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
-    </row>
-    <row r="42" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="F41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>2</v>
       </c>
-      <c r="B42" s="13" t="s">
+      <c r="B42" s="9" t="s">
         <v>49</v>
       </c>
       <c r="C42" s="5">
@@ -6227,8 +6448,11 @@
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
-    </row>
-    <row r="43" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="F42">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>3</v>
       </c>
@@ -6241,9 +6465,9 @@
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
     </row>
-    <row r="44" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
-      <c r="B44" s="13" t="s">
+      <c r="B44" s="9" t="s">
         <v>27</v>
       </c>
       <c r="C44" s="5">
@@ -6252,8 +6476,8 @@
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
     </row>
-    <row r="45" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" s="12" t="s">
+    <row r="45" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A45" s="8" t="s">
         <v>50</v>
       </c>
       <c r="B45" s="4"/>
@@ -6261,7 +6485,7 @@
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
     </row>
-    <row r="46" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>8</v>
       </c>
@@ -6278,11 +6502,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>1</v>
       </c>
-      <c r="B47" s="13" t="s">
+      <c r="B47" s="9" t="s">
         <v>51</v>
       </c>
       <c r="C47" s="5">
@@ -6291,11 +6515,11 @@
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
     </row>
-    <row r="48" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>2</v>
       </c>
-      <c r="B48" s="13" t="s">
+      <c r="B48" s="9" t="s">
         <v>52</v>
       </c>
       <c r="C48" s="5">
@@ -6304,11 +6528,11 @@
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
     </row>
-    <row r="49" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>3</v>
       </c>
-      <c r="B49" s="13" t="s">
+      <c r="B49" s="9" t="s">
         <v>53</v>
       </c>
       <c r="C49" s="5">
@@ -6317,11 +6541,11 @@
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
     </row>
-    <row r="50" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>4</v>
       </c>
-      <c r="B50" s="13" t="s">
+      <c r="B50" s="9" t="s">
         <v>54</v>
       </c>
       <c r="C50" s="5">
@@ -6330,11 +6554,11 @@
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
     </row>
-    <row r="51" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>5</v>
       </c>
-      <c r="B51" s="13" t="s">
+      <c r="B51" s="9" t="s">
         <v>15</v>
       </c>
       <c r="C51" s="5">
@@ -6343,9 +6567,9 @@
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
     </row>
-    <row r="52" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="5"/>
-      <c r="B52" s="13" t="s">
+      <c r="B52" s="9" t="s">
         <v>55</v>
       </c>
       <c r="C52" s="5">
@@ -6354,8 +6578,8 @@
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
     </row>
-    <row r="53" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A53" s="12" t="s">
+    <row r="53" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A53" s="8" t="s">
         <v>61</v>
       </c>
       <c r="B53" s="4"/>
@@ -6363,7 +6587,7 @@
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
     </row>
-    <row r="54" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>8</v>
       </c>
@@ -6380,11 +6604,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>1</v>
       </c>
-      <c r="B55" s="13" t="s">
+      <c r="B55" s="9" t="s">
         <v>56</v>
       </c>
       <c r="C55" s="5">
@@ -6393,15 +6617,19 @@
       <c r="D55" s="5">
         <v>2</v>
       </c>
-      <c r="E55" s="13" t="s">
+      <c r="E55" s="9" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="F55">
+        <f>18/5</f>
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <v>2</v>
       </c>
-      <c r="B56" s="13" t="s">
+      <c r="B56" s="9" t="s">
         <v>59</v>
       </c>
       <c r="C56" s="5">
@@ -6410,15 +6638,19 @@
       <c r="D56" s="5">
         <v>2</v>
       </c>
-      <c r="E56" s="13" t="s">
+      <c r="E56" s="9" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="F56">
+        <f>18/5</f>
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>3</v>
       </c>
-      <c r="B57" s="13" t="s">
+      <c r="B57" s="9" t="s">
         <v>57</v>
       </c>
       <c r="C57" s="5">
@@ -6427,15 +6659,19 @@
       <c r="D57" s="5">
         <v>3</v>
       </c>
-      <c r="E57" s="13" t="s">
+      <c r="E57" s="9" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="F57">
+        <f>18/5</f>
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <v>4</v>
       </c>
-      <c r="B58" s="13" t="s">
+      <c r="B58" s="9" t="s">
         <v>58</v>
       </c>
       <c r="C58" s="5">
@@ -6443,12 +6679,16 @@
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="5"/>
-    </row>
-    <row r="59" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="F58">
+        <f>18/5</f>
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <v>5</v>
       </c>
-      <c r="B59" s="13" t="s">
+      <c r="B59" s="9" t="s">
         <v>15</v>
       </c>
       <c r="C59" s="5">
@@ -6456,10 +6696,14 @@
       </c>
       <c r="D59" s="5"/>
       <c r="E59" s="5"/>
-    </row>
-    <row r="60" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="F59">
+        <f>18/5</f>
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="5"/>
-      <c r="B60" s="13" t="s">
+      <c r="B60" s="9" t="s">
         <v>60</v>
       </c>
       <c r="C60" s="5">
@@ -6468,8 +6712,8 @@
       <c r="D60" s="5"/>
       <c r="E60" s="5"/>
     </row>
-    <row r="61" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A61" s="12" t="s">
+    <row r="61" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A61" s="8" t="s">
         <v>62</v>
       </c>
       <c r="B61" s="4"/>
@@ -6477,7 +6721,7 @@
       <c r="D61" s="4"/>
       <c r="E61" s="4"/>
     </row>
-    <row r="62" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>8</v>
       </c>
@@ -6494,11 +6738,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="5">
         <v>1</v>
       </c>
-      <c r="B63" s="13" t="s">
+      <c r="B63" s="9" t="s">
         <v>63</v>
       </c>
       <c r="C63" s="5">
@@ -6507,15 +6751,15 @@
       <c r="D63" s="5">
         <v>2</v>
       </c>
-      <c r="E63" s="13" t="s">
+      <c r="E63" s="9" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
         <v>2</v>
       </c>
-      <c r="B64" s="13" t="s">
+      <c r="B64" s="9" t="s">
         <v>64</v>
       </c>
       <c r="C64" s="5">
@@ -6524,11 +6768,11 @@
       <c r="D64" s="5"/>
       <c r="E64" s="5"/>
     </row>
-    <row r="65" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
         <v>3</v>
       </c>
-      <c r="B65" s="13" t="s">
+      <c r="B65" s="9" t="s">
         <v>15</v>
       </c>
       <c r="C65" s="5">
@@ -6537,9 +6781,9 @@
       <c r="D65" s="5"/>
       <c r="E65" s="5"/>
     </row>
-    <row r="66" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="5"/>
-      <c r="B66" s="13" t="s">
+      <c r="B66" s="9" t="s">
         <v>16</v>
       </c>
       <c r="C66" s="5">
@@ -6547,9 +6791,12 @@
       </c>
       <c r="D66" s="5"/>
       <c r="E66" s="5"/>
-    </row>
-    <row r="67" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A67" s="12" t="s">
+      <c r="F66">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A67" s="8" t="s">
         <v>65</v>
       </c>
       <c r="B67" s="4"/>
@@ -6557,7 +6804,7 @@
       <c r="D67" s="4"/>
       <c r="E67" s="4"/>
     </row>
-    <row r="68" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>8</v>
       </c>
@@ -6574,11 +6821,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="5">
         <v>1</v>
       </c>
-      <c r="B69" s="14" t="s">
+      <c r="B69" s="10" t="s">
         <v>66</v>
       </c>
       <c r="C69" s="5">
@@ -6587,11 +6834,11 @@
       <c r="D69" s="5"/>
       <c r="E69" s="5"/>
     </row>
-    <row r="70" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
         <v>2</v>
       </c>
-      <c r="B70" s="13" t="s">
+      <c r="B70" s="9" t="s">
         <v>67</v>
       </c>
       <c r="C70" s="5">
@@ -6600,11 +6847,11 @@
       <c r="D70" s="5"/>
       <c r="E70" s="5"/>
     </row>
-    <row r="71" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="5">
         <v>3</v>
       </c>
-      <c r="B71" s="13" t="s">
+      <c r="B71" s="9" t="s">
         <v>15</v>
       </c>
       <c r="C71" s="5">
@@ -6613,9 +6860,9 @@
       <c r="D71" s="5"/>
       <c r="E71" s="5"/>
     </row>
-    <row r="72" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="5"/>
-      <c r="B72" s="13" t="s">
+      <c r="B72" s="9" t="s">
         <v>55</v>
       </c>
       <c r="C72" s="5">

</xml_diff>